<commit_message>
Added to Data Dictionary
Added contents, whether it's a PK/FK, and whether it's required
</commit_message>
<xml_diff>
--- a/Autoparts Data Dictionary.xlsx
+++ b/Autoparts Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\GitHub\database-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BBE5F2-A116-473D-8923-9B3AA48BA385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A986FA4-1C17-4B48-BCCE-15B28D5F27B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="115">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -111,9 +111,6 @@
     <t>sp_NumSales</t>
   </si>
   <si>
-    <t>sp_Comission</t>
-  </si>
-  <si>
     <t>sp_YTDSales</t>
   </si>
   <si>
@@ -133,6 +130,246 @@
   </si>
   <si>
     <t>Product List</t>
+  </si>
+  <si>
+    <t>prod_ID</t>
+  </si>
+  <si>
+    <t>prodList_Num</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>prod_isUsed</t>
+  </si>
+  <si>
+    <t>prod_Name</t>
+  </si>
+  <si>
+    <t>prod_InvAmount</t>
+  </si>
+  <si>
+    <t>prod_Price</t>
+  </si>
+  <si>
+    <t>prod_Type</t>
+  </si>
+  <si>
+    <t>prod_ModNum</t>
+  </si>
+  <si>
+    <t>prod_Supplier</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>cus_Name</t>
+  </si>
+  <si>
+    <t>cus_Address</t>
+  </si>
+  <si>
+    <t>cus_Type</t>
+  </si>
+  <si>
+    <t>cus_Income</t>
+  </si>
+  <si>
+    <t>cus_Phone</t>
+  </si>
+  <si>
+    <t>cus_NumVec</t>
+  </si>
+  <si>
+    <t>cus_Insur</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>bus_Category</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>home_MarrStat</t>
+  </si>
+  <si>
+    <t>home_Gender</t>
+  </si>
+  <si>
+    <t>home_Age</t>
+  </si>
+  <si>
+    <t>home_NumRes</t>
+  </si>
+  <si>
+    <t>PK, FK</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Region's ID</t>
+  </si>
+  <si>
+    <t>Employee's ID</t>
+  </si>
+  <si>
+    <t>Store's ID</t>
+  </si>
+  <si>
+    <t>Name for Region</t>
+  </si>
+  <si>
+    <t>Region's Zip Code</t>
+  </si>
+  <si>
+    <t>Manager's employee ID</t>
+  </si>
+  <si>
+    <t>Store region ID</t>
+  </si>
+  <si>
+    <t>The number of salespersons at a store</t>
+  </si>
+  <si>
+    <t>Store's total sales</t>
+  </si>
+  <si>
+    <t>City store is located in</t>
+  </si>
+  <si>
+    <t>Store employee works at</t>
+  </si>
+  <si>
+    <t>Employee's email</t>
+  </si>
+  <si>
+    <t>Employee's salary</t>
+  </si>
+  <si>
+    <t>Employee's job</t>
+  </si>
+  <si>
+    <t>Salesperson's employee ID</t>
+  </si>
+  <si>
+    <t>Number of sales this year</t>
+  </si>
+  <si>
+    <t>sp_Commission</t>
+  </si>
+  <si>
+    <t>Commission rate for salesperson</t>
+  </si>
+  <si>
+    <t>Salesperson's year-to-date sales</t>
+  </si>
+  <si>
+    <t>Transaction's ID</t>
+  </si>
+  <si>
+    <t>Employee who performed the transaction</t>
+  </si>
+  <si>
+    <t>Customer who paid for the transaction</t>
+  </si>
+  <si>
+    <t>Store transaction took place at</t>
+  </si>
+  <si>
+    <t>Date of transaction</t>
+  </si>
+  <si>
+    <t>Total price for transaction</t>
+  </si>
+  <si>
+    <t>Transaction ID</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Amount of product included in transaction</t>
+  </si>
+  <si>
+    <t>Product's ID</t>
+  </si>
+  <si>
+    <t>Whether product is new or used</t>
+  </si>
+  <si>
+    <t>Amount in inventory</t>
+  </si>
+  <si>
+    <t>Product type</t>
+  </si>
+  <si>
+    <t>Product price</t>
+  </si>
+  <si>
+    <t>Product's name</t>
+  </si>
+  <si>
+    <t>Product's Model Number</t>
+  </si>
+  <si>
+    <t>Product's Supplier</t>
+  </si>
+  <si>
+    <t>Customer's ID</t>
+  </si>
+  <si>
+    <t>Customer's Name</t>
+  </si>
+  <si>
+    <t>Customer's Home/Business address</t>
+  </si>
+  <si>
+    <t>Customer type (Home/Business)</t>
+  </si>
+  <si>
+    <t>Customer's annual income</t>
+  </si>
+  <si>
+    <t>Customer's phone number</t>
+  </si>
+  <si>
+    <t>Numer of vehicles customer owns</t>
+  </si>
+  <si>
+    <t>Customer's Insurance Provider</t>
+  </si>
+  <si>
+    <t>Business's customer ID</t>
+  </si>
+  <si>
+    <t>Business Category</t>
+  </si>
+  <si>
+    <t>bus_NumEmp</t>
+  </si>
+  <si>
+    <t>Number of employees the business has</t>
+  </si>
+  <si>
+    <t>Person's Customer ID</t>
+  </si>
+  <si>
+    <t>Person's marriage status</t>
+  </si>
+  <si>
+    <t>Person's gender</t>
+  </si>
+  <si>
+    <t>Person's age</t>
+  </si>
+  <si>
+    <t>Number of people in person's home</t>
   </si>
 </sst>
 </file>
@@ -188,8 +425,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{525CC2C1-F61E-480D-A8FE-067540B6740E}" name="Table2" displayName="Table2" ref="A1:I40" totalsRowShown="0">
-  <autoFilter ref="A1:I40" xr:uid="{525CC2C1-F61E-480D-A8FE-067540B6740E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{525CC2C1-F61E-480D-A8FE-067540B6740E}" name="Table2" displayName="Table2" ref="A1:I53" totalsRowShown="0">
+  <autoFilter ref="A1:I53" xr:uid="{525CC2C1-F61E-480D-A8FE-067540B6740E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -478,26 +715,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="36.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.26953125" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,13 +763,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
@@ -540,12 +780,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>13</v>
       </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -554,23 +797,38 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
@@ -578,12 +836,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>13</v>
       </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
@@ -592,10 +853,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
       <c r="G8" t="s">
         <v>12</v>
       </c>
@@ -606,108 +870,592 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
       <c r="B21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
         <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>100</v>
+      </c>
+      <c r="G40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+      <c r="G41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>103</v>
+      </c>
+      <c r="G42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="G43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
+        <v>105</v>
+      </c>
+      <c r="G44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
+        <v>60</v>
+      </c>
+      <c r="I46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>107</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="G49" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s">
+        <v>60</v>
+      </c>
+      <c r="I49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" t="s">
+        <v>111</v>
+      </c>
+      <c r="G50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" t="s">
+        <v>112</v>
+      </c>
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+      <c r="G52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" t="s">
+        <v>114</v>
+      </c>
+      <c r="G53" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Autoparts Data Dictionary.xlsx
</commit_message>
<xml_diff>
--- a/Autoparts Data Dictionary.xlsx
+++ b/Autoparts Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\GitHub\database-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F9F049-A068-493A-8D81-2E6B3AB943B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF277D1-6119-4FB4-8CA9-6912AF273FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -842,7 +842,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Data Dictionary and ERD match
Data Dictionary and ERD should now match.
</commit_message>
<xml_diff>
--- a/Autoparts Data Dictionary.xlsx
+++ b/Autoparts Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\GitHub\database-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C61B865-F8F3-4D17-97FE-F5E5CBF38235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612B2AE4-5045-4BB4-B9E9-0ABEA66D11D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Removed NOT NULL constraint from FKs
Removed NOT NULL constraint from FKs and requirement from data dictionary (It was causing initially filling the tables to be impossible)
</commit_message>
<xml_diff>
--- a/Autoparts Data Dictionary.xlsx
+++ b/Autoparts Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\GitHub\database-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612B2AE4-5045-4BB4-B9E9-0ABEA66D11D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497E3DA3-F5FB-4002-B5DA-550029C98F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>10000-99999</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -1081,7 +1081,7 @@
         <v>10000-99999</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
@@ -1111,7 +1111,7 @@
         <v>10000-99999</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H8" t="s">
         <v>12</v>
@@ -1217,7 +1217,7 @@
         <v>10000-99999</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H13" t="s">
         <v>12</v>
@@ -1493,7 +1493,7 @@
         <v>84</v>
       </c>
       <c r="G25" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1711,15 +1711,15 @@
         <v>53</v>
       </c>
       <c r="D36" s="15" t="str">
-        <f>D27</f>
+        <f t="shared" ref="D36:F37" si="0">D27</f>
         <v>CHAR(5)</v>
       </c>
       <c r="E36" s="16">
-        <f>E27</f>
+        <f t="shared" si="0"/>
         <v>99999</v>
       </c>
       <c r="F36" s="17" t="str">
-        <f>F27</f>
+        <f t="shared" si="0"/>
         <v>10000-99999</v>
       </c>
       <c r="G36" s="13" t="s">
@@ -1742,15 +1742,15 @@
         <v>56</v>
       </c>
       <c r="D37" s="15" t="str">
-        <f>D28</f>
+        <f t="shared" si="0"/>
         <v>NUMBER(1)</v>
       </c>
       <c r="E37" s="16">
-        <f>E28</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F37" s="17" t="str">
-        <f>F28</f>
+        <f t="shared" si="0"/>
         <v>0-1</v>
       </c>
       <c r="G37" s="13" t="s">

</xml_diff>

<commit_message>
Added employee first and last name fields
Added employee first name and last name.
</commit_message>
<xml_diff>
--- a/Autoparts Data Dictionary.xlsx
+++ b/Autoparts Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\GitHub\database-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497E3DA3-F5FB-4002-B5DA-550029C98F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B6DBC4-6AA1-496C-830F-B1D16206B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="144">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -452,6 +452,18 @@
   </si>
   <si>
     <t>home_NumResidents</t>
+  </si>
+  <si>
+    <t>employee_last</t>
+  </si>
+  <si>
+    <t>employee_first</t>
+  </si>
+  <si>
+    <t>Employee's first name</t>
+  </si>
+  <si>
+    <t>Employee's last name</t>
   </si>
 </sst>
 </file>
@@ -603,8 +615,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{525CC2C1-F61E-480D-A8FE-067540B6740E}" name="Table2" displayName="Table2" ref="A1:I54" totalsRowShown="0">
-  <autoFilter ref="A1:I54" xr:uid="{525CC2C1-F61E-480D-A8FE-067540B6740E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{525CC2C1-F61E-480D-A8FE-067540B6740E}" name="Table2" displayName="Table2" ref="A1:I56" totalsRowShown="0">
+  <autoFilter ref="A1:I56" xr:uid="{525CC2C1-F61E-480D-A8FE-067540B6740E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -893,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,409 +1238,409 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" s="9">
-        <v>9999999.9900000002</v>
-      </c>
-      <c r="F15" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="E14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="9">
+        <v>9999999.9900000002</v>
+      </c>
+      <c r="F17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>113</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B19" t="str">
         <f>B12</f>
         <v>employee_ID</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="2" t="str">
+      <c r="D19" s="2" t="str">
         <f>D12</f>
         <v>CHAR(5)</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E19" s="3">
         <f>E12</f>
         <v>99999</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
         <v>29</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I19" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E18" s="10">
-        <v>9999</v>
-      </c>
-      <c r="G18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="9">
-        <v>9999999.9900000002</v>
-      </c>
-      <c r="G19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="10">
+        <v>9999</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="9">
+        <v>9999999.9900000002</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E22" s="9">
         <v>9999999.9900000002</v>
       </c>
-      <c r="G20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>114</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E23" s="3">
         <v>99999</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" t="str">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="str">
         <f>B12</f>
         <v>employee_ID</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="2" t="str">
+      <c r="D24" s="2" t="str">
         <f>D12</f>
         <v>CHAR(5)</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E24" s="4">
         <f>E12</f>
         <v>99999</v>
       </c>
-      <c r="F22" t="str">
+      <c r="F24" t="str">
         <f>F12</f>
         <v>10000-99999</v>
       </c>
-      <c r="G22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
         <v>12</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" t="str">
-        <f>B39</f>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <f>B41</f>
         <v>customer_ID</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="2" t="str">
-        <f>D39</f>
+      <c r="D25" s="2" t="str">
+        <f>D41</f>
         <v>CHAR(5)</v>
       </c>
-      <c r="E23" s="4">
-        <f>E39</f>
+      <c r="E25" s="4">
+        <f>E41</f>
         <v>99999</v>
       </c>
-      <c r="F23" t="str">
-        <f>F39</f>
+      <c r="F25" t="str">
+        <f>F41</f>
         <v>10000-99999</v>
       </c>
-      <c r="G23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
         <v>12</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" t="str">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
         <f>B6</f>
         <v>store_ID</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="2" t="str">
+      <c r="D26" s="2" t="str">
         <f>D6</f>
         <v>CHAR(5)</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E26" s="4">
         <f>E6</f>
         <v>99999</v>
       </c>
-      <c r="F24" t="str">
+      <c r="F26" t="str">
         <f>F6</f>
         <v>10000-99999</v>
       </c>
-      <c r="G24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
         <v>12</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>116</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="9">
-        <v>9999999.9900000002</v>
-      </c>
-      <c r="G26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" s="3">
-        <v>99999</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="G27" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" s="6">
-        <v>9</v>
-      </c>
-      <c r="F28" t="s">
-        <v>105</v>
+        <v>51</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="9">
+        <v>9999999.9900000002</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="3">
+        <v>99999</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29"/>
-      <c r="G29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29"/>
-      <c r="I29"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="3">
-        <v>9999</v>
+        <v>56</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="6">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>105</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31"/>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="9">
-        <v>9999999.9900000002</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31"/>
       <c r="G31" t="s">
         <v>30</v>
       </c>
+      <c r="H31"/>
+      <c r="I31"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>81</v>
+        <v>57</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="3">
+        <v>9999</v>
       </c>
       <c r="G32" t="s">
         <v>11</v>
@@ -1636,27 +1648,27 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>81</v>
+        <v>59</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="9">
+        <v>9999999.9900000002</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>80</v>
@@ -1665,216 +1677,216 @@
         <v>81</v>
       </c>
       <c r="G34" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="13" t="str">
-        <f>B21</f>
+      <c r="B37" s="13" t="str">
+        <f>B23</f>
         <v>transaction_ID</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C37" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="15" t="str">
-        <f>D21</f>
+      <c r="D37" s="15" t="str">
+        <f>D23</f>
         <v>CHAR(5)</v>
       </c>
-      <c r="E35" s="16">
-        <f>E21</f>
+      <c r="E37" s="16">
+        <f>E23</f>
         <v>99999</v>
       </c>
-      <c r="F35" s="13" t="str">
-        <f>F21</f>
+      <c r="F37" s="13" t="str">
+        <f>F23</f>
         <v>10000-99999</v>
       </c>
-      <c r="G35" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="13" t="s">
+      <c r="G37" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="I37" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="13" t="str">
-        <f>B27</f>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="13" t="str">
+        <f>B29</f>
         <v>product_ID</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C38" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="15" t="str">
-        <f t="shared" ref="D36:F37" si="0">D27</f>
+      <c r="D38" s="15" t="str">
+        <f t="shared" ref="D38:F39" si="0">D29</f>
         <v>CHAR(5)</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E38" s="16">
         <f t="shared" si="0"/>
         <v>99999</v>
       </c>
-      <c r="F36" s="17" t="str">
+      <c r="F38" s="17" t="str">
         <f t="shared" si="0"/>
         <v>10000-99999</v>
       </c>
-      <c r="G36" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="13" t="s">
+      <c r="G38" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I36" s="14" t="s">
+      <c r="I38" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="13" t="str">
-        <f>B28</f>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="13" t="str">
+        <f>B30</f>
         <v>product_isUsed</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C39" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="15" t="str">
+      <c r="D39" s="15" t="str">
         <f t="shared" si="0"/>
         <v>NUMBER(1)</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E39" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F37" s="17" t="str">
+      <c r="F39" s="17" t="str">
         <f t="shared" si="0"/>
         <v>0-1</v>
       </c>
-      <c r="G37" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="13" t="s">
+      <c r="G39" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I39" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C40" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D40" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E40" s="17">
         <v>9999</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F40" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="G38" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="14"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="G40" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="13"/>
+      <c r="I40" s="14"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>24</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>115</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E41" s="3">
         <v>99999</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" t="s">
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>128</v>
-      </c>
-      <c r="C41" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G41" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" s="9">
-        <v>9999999.9900000002</v>
+        <v>64</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="G42" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="G43" t="s">
         <v>30</v>
@@ -1882,16 +1894,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E44" s="4">
-        <v>99999</v>
+        <v>85</v>
+      </c>
+      <c r="E44" s="9">
+        <v>9999999.9900000002</v>
       </c>
       <c r="G44" t="s">
         <v>30</v>
@@ -1899,187 +1911,187 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="G45" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>88</v>
+        <v>132</v>
+      </c>
+      <c r="E46" s="4">
+        <v>99999</v>
       </c>
       <c r="G46" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47" t="str">
-        <f>B39</f>
-        <v>customer_ID</v>
+      <c r="B47" t="s">
+        <v>133</v>
       </c>
       <c r="C47" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="2" t="str">
-        <f>D39</f>
-        <v>CHAR(5)</v>
-      </c>
-      <c r="E47" s="4">
-        <f>E39</f>
-        <v>99999</v>
-      </c>
-      <c r="F47" t="str">
-        <f>F39</f>
-        <v>10000-99999</v>
+        <v>70</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="G47" t="s">
         <v>11</v>
-      </c>
-      <c r="H47" t="s">
-        <v>29</v>
-      </c>
-      <c r="I47" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" t="str">
+        <f>B41</f>
+        <v>customer_ID</v>
+      </c>
+      <c r="C49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="2" t="str">
+        <f>D41</f>
+        <v>CHAR(5)</v>
+      </c>
+      <c r="E49" s="4">
+        <f>E41</f>
+        <v>99999</v>
+      </c>
+      <c r="F49" t="str">
+        <f>F41</f>
+        <v>10000-99999</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" t="s">
+        <v>29</v>
+      </c>
+      <c r="I49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>135</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E49" s="4">
-        <v>99999</v>
-      </c>
-      <c r="F49" t="s">
-        <v>101</v>
-      </c>
-      <c r="G49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" t="str">
-        <f>B39</f>
-        <v>customer_ID</v>
-      </c>
-      <c r="C50" t="s">
-        <v>74</v>
-      </c>
-      <c r="D50" s="2" t="str">
-        <f>D39</f>
-        <v>CHAR(5)</v>
-      </c>
-      <c r="E50" s="4">
-        <f>E39</f>
-        <v>99999</v>
-      </c>
-      <c r="F50" t="str">
-        <f>F39</f>
-        <v>10000-99999</v>
-      </c>
       <c r="G50" t="s">
         <v>11</v>
-      </c>
-      <c r="H50" t="s">
-        <v>29</v>
-      </c>
-      <c r="I50" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>98</v>
+        <v>73</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="4">
+        <v>99999</v>
+      </c>
+      <c r="F51" t="s">
+        <v>101</v>
       </c>
       <c r="G51" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>27</v>
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" t="str">
+        <f>B41</f>
+        <v>customer_ID</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>98</v>
+        <v>74</v>
+      </c>
+      <c r="D52" s="2" t="str">
+        <f>D41</f>
+        <v>CHAR(5)</v>
+      </c>
+      <c r="E52" s="4">
+        <f>E41</f>
+        <v>99999</v>
+      </c>
+      <c r="F52" t="str">
+        <f>F41</f>
+        <v>10000-99999</v>
       </c>
       <c r="G52" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="H52" t="s">
+        <v>29</v>
+      </c>
+      <c r="I52" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E53" s="3">
-        <v>999</v>
+        <v>97</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="G53" t="s">
         <v>30</v>
@@ -2087,25 +2099,59 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" s="3">
+        <v>999</v>
+      </c>
+      <c r="G55" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>139</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>78</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D56" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E56" s="3">
         <v>999</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G56" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E14" r:id="rId1" xr:uid="{C47EC26E-BF03-4AA8-9F39-B69952F2C995}"/>
+    <hyperlink ref="E16" r:id="rId1" xr:uid="{C47EC26E-BF03-4AA8-9F39-B69952F2C995}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Replaced CHAR with NUMBER
Changed the datatype of PKs and a few other attributes to be NUMBER instead of CHAR since it fits the data better.
</commit_message>
<xml_diff>
--- a/Autoparts Data Dictionary.xlsx
+++ b/Autoparts Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\GitHub\database-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B6DBC4-6AA1-496C-830F-B1D16206B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F2EB09-F17D-42AB-BCA1-1DCF9A0A126A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="141">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -271,18 +271,12 @@
     <t>Number of people in person's home</t>
   </si>
   <si>
-    <t>CHAR(5)</t>
-  </si>
-  <si>
     <t>VARCHAR(20)</t>
   </si>
   <si>
     <t>Xxxxxxxx</t>
   </si>
   <si>
-    <t>Number(9,2)</t>
-  </si>
-  <si>
     <t>DATE</t>
   </si>
   <si>
@@ -301,9 +295,6 @@
     <t>xx</t>
   </si>
   <si>
-    <t>Employee's job title/position</t>
-  </si>
-  <si>
     <t>Number of sales/transactions this year</t>
   </si>
   <si>
@@ -313,15 +304,9 @@
     <t>Total amount of sales (Year-To-Date)</t>
   </si>
   <si>
-    <t>NUMBER(4,0)</t>
-  </si>
-  <si>
     <t>VARCHAR(30)</t>
   </si>
   <si>
-    <t>CHAR(10)</t>
-  </si>
-  <si>
     <t>(999) 999-9999</t>
   </si>
   <si>
@@ -343,9 +328,6 @@
     <t>1-9999</t>
   </si>
   <si>
-    <t>NUMBER(3,0)</t>
-  </si>
-  <si>
     <t>NUMBER(1)</t>
   </si>
   <si>
@@ -464,6 +446,15 @@
   </si>
   <si>
     <t>Employee's last name</t>
+  </si>
+  <si>
+    <t>NUMBER(10)</t>
+  </si>
+  <si>
+    <t>NUMBER(3)</t>
+  </si>
+  <si>
+    <t>Employee's job title/position (subtype)</t>
   </si>
 </sst>
 </file>
@@ -907,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,19 +949,19 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>79</v>
+      <c r="D2" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="E2" s="3">
         <v>99999</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -989,7 +980,7 @@
       </c>
       <c r="D3" s="2" t="str">
         <f>D12</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E3" s="3">
         <f>E12</f>
@@ -1011,16 +1002,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="G4" t="s">
         <v>30</v>
@@ -1028,19 +1019,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>79</v>
+      <c r="D5" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="E5" s="3">
         <v>99999</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -1056,14 +1047,14 @@
       <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>79</v>
+      <c r="D6" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="E6" s="3">
         <v>99999</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -1082,7 +1073,7 @@
       </c>
       <c r="D7" s="2" t="str">
         <f>D12</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E7" s="3">
         <f>E12</f>
@@ -1112,7 +1103,7 @@
       </c>
       <c r="D8" s="2" t="str">
         <f>D2</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E8" s="4">
         <f>E2</f>
@@ -1139,8 +1130,8 @@
       <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>79</v>
+      <c r="D9" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="E9" s="4">
         <v>99999</v>
@@ -1151,13 +1142,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E10" s="5">
         <v>9999999.9900000002</v>
@@ -1174,10 +1165,10 @@
         <v>40</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G11" t="s">
         <v>30</v>
@@ -1188,19 +1179,19 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>79</v>
+      <c r="D12" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="E12" s="3">
         <v>99999</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -1218,7 +1209,7 @@
       </c>
       <c r="D13" s="2" t="str">
         <f>D6</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E13" s="4">
         <f>E6</f>
@@ -1240,16 +1231,16 @@
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>30</v>
@@ -1257,16 +1248,16 @@
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>30</v>
@@ -1274,16 +1265,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G16" t="s">
         <v>30</v>
@@ -1291,19 +1282,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E17" s="9">
         <v>9999999.9900000002</v>
       </c>
       <c r="F17" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G17" t="s">
         <v>30</v>
@@ -1311,16 +1302,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G18" t="s">
         <v>30</v>
@@ -1339,14 +1330,14 @@
       </c>
       <c r="D19" s="2" t="str">
         <f>D12</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E19" s="3">
         <f>E12</f>
         <v>99999</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -1363,10 +1354,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E20" s="10">
         <v>9999</v>
@@ -1380,10 +1371,10 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E21" s="9">
         <v>9999999.9900000002</v>
@@ -1397,10 +1388,10 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E22" s="9">
         <v>9999999.9900000002</v>
@@ -1414,19 +1405,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>79</v>
+      <c r="D23" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="E23" s="3">
         <v>99999</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
@@ -1445,7 +1436,7 @@
       </c>
       <c r="D24" s="2" t="str">
         <f>D12</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E24" s="4">
         <f>E12</f>
@@ -1475,7 +1466,7 @@
       </c>
       <c r="D25" s="2" t="str">
         <f>D41</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E25" s="4">
         <f>E41</f>
@@ -1505,7 +1496,7 @@
       </c>
       <c r="D26" s="2" t="str">
         <f>D6</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E26" s="4">
         <f>E6</f>
@@ -1527,16 +1518,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C27" t="s">
         <v>50</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G27" t="s">
         <v>30</v>
@@ -1544,13 +1535,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C28" t="s">
         <v>51</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E28" s="9">
         <v>9999999.9900000002</v>
@@ -1564,19 +1555,19 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
         <v>55</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="E29" s="3">
         <v>99999</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G29" t="s">
         <v>11</v>
@@ -1587,19 +1578,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
         <v>56</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E30" s="6">
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
@@ -1611,16 +1602,16 @@
     <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C31" t="s">
         <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="F31"/>
       <c r="G31" t="s">
@@ -1631,13 +1622,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
         <v>57</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="E32" s="3">
         <v>9999</v>
@@ -1648,13 +1639,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>82</v>
+      <c r="D33" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="E33" s="9">
         <v>9999999.9900000002</v>
@@ -1665,16 +1656,16 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C34" t="s">
         <v>58</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G34" t="s">
         <v>11</v>
@@ -1682,16 +1673,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
         <v>61</v>
       </c>
       <c r="D35" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="G35" t="s">
         <v>11</v>
@@ -1699,16 +1690,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C36" t="s">
         <v>62</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G36" t="s">
         <v>30</v>
@@ -1727,7 +1718,7 @@
       </c>
       <c r="D37" s="15" t="str">
         <f>D23</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E37" s="16">
         <f>E23</f>
@@ -1758,7 +1749,7 @@
       </c>
       <c r="D38" s="15" t="str">
         <f t="shared" ref="D38:F39" si="0">D29</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E38" s="16">
         <f t="shared" si="0"/>
@@ -1812,19 +1803,19 @@
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>54</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="E40" s="17">
         <v>9999</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>11</v>
@@ -1837,19 +1828,19 @@
         <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>79</v>
+      <c r="D41" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="E41" s="3">
         <v>99999</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G41" t="s">
         <v>11</v>
@@ -1860,16 +1851,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
         <v>64</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G42" t="s">
         <v>11</v>
@@ -1877,16 +1868,16 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
         <v>65</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G43" t="s">
         <v>30</v>
@@ -1894,13 +1885,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
         <v>67</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E44" s="9">
         <v>9999999.9900000002</v>
@@ -1911,16 +1902,16 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
         <v>68</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G45" t="s">
         <v>30</v>
@@ -1928,13 +1919,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C46" t="s">
         <v>69</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E46" s="4">
         <v>99999</v>
@@ -1945,16 +1936,16 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C47" t="s">
         <v>70</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G47" t="s">
         <v>11</v>
@@ -1962,16 +1953,16 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
         <v>66</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G48" t="s">
         <v>11</v>
@@ -1990,7 +1981,7 @@
       </c>
       <c r="D49" s="2" t="str">
         <f>D41</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E49" s="4">
         <f>E41</f>
@@ -2012,16 +2003,16 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C50" t="s">
         <v>72</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G50" t="s">
         <v>11</v>
@@ -2029,19 +2020,19 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C51" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>79</v>
+      <c r="D51" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="E51" s="4">
         <v>99999</v>
       </c>
       <c r="F51" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G51" t="s">
         <v>30</v>
@@ -2060,7 +2051,7 @@
       </c>
       <c r="D52" s="2" t="str">
         <f>D41</f>
-        <v>CHAR(5)</v>
+        <v>NUMBER(5)</v>
       </c>
       <c r="E52" s="4">
         <f>E41</f>
@@ -2082,16 +2073,16 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
         <v>75</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G53" t="s">
         <v>30</v>
@@ -2105,10 +2096,10 @@
         <v>76</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G54" t="s">
         <v>30</v>
@@ -2122,7 +2113,7 @@
         <v>77</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="E55" s="3">
         <v>999</v>
@@ -2133,13 +2124,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C56" t="s">
         <v>78</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="E56" s="3">
         <v>999</v>

</xml_diff>

<commit_message>
Added FK constraint to store table
</commit_message>
<xml_diff>
--- a/Autoparts Data Dictionary.xlsx
+++ b/Autoparts Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\GitHub\database-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428B6146-362E-4C06-9A93-D1BA127129A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CC2F0A-A6D0-4267-8668-FFD9CDFAFE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -319,9 +319,6 @@
     <t>10000-99999</t>
   </si>
   <si>
-    <t>10000.00-999999.99</t>
-  </si>
-  <si>
     <t>1-99999</t>
   </si>
   <si>
@@ -436,12 +433,6 @@
     <t>home_NumResidents</t>
   </si>
   <si>
-    <t>employee_last</t>
-  </si>
-  <si>
-    <t>employee_first</t>
-  </si>
-  <si>
     <t>Employee's first name</t>
   </si>
   <si>
@@ -455,6 +446,15 @@
   </si>
   <si>
     <t>Employee's job title/position (subtype)</t>
+  </si>
+  <si>
+    <t>employee_First</t>
+  </si>
+  <si>
+    <t>employee_Last</t>
+  </si>
+  <si>
+    <t>&gt;=10000</t>
   </si>
 </sst>
 </file>
@@ -899,7 +899,7 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,13 +949,13 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E2" s="3">
         <v>99999</v>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
@@ -1019,13 +1019,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E5" s="3">
         <v>99999</v>
@@ -1048,7 +1048,7 @@
         <v>33</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E6" s="3">
         <v>99999</v>
@@ -1131,7 +1131,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E9" s="4">
         <v>99999</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1179,13 +1179,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E12" s="3">
         <v>99999</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>79</v>
@@ -1248,10 +1248,10 @@
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>79</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
         <v>42</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
         <v>43</v>
@@ -1294,7 +1294,7 @@
         <v>9999999.9900000002</v>
       </c>
       <c r="F17" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="G17" t="s">
         <v>30</v>
@@ -1302,10 +1302,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>85</v>
@@ -1357,7 +1357,7 @@
         <v>87</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E20" s="10">
         <v>9999</v>
@@ -1405,13 +1405,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E23" s="3">
         <v>99999</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
         <v>50</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
         <v>51</v>
@@ -1555,13 +1555,13 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
         <v>55</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E29" s="3">
         <v>99999</v>
@@ -1578,19 +1578,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C30" t="s">
         <v>56</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30" s="6">
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
@@ -1602,7 +1602,7 @@
     <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31" t="s">
         <v>60</v>
@@ -1622,13 +1622,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C32" t="s">
         <v>57</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E32" s="3">
         <v>9999</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
         <v>59</v>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
         <v>58</v>
@@ -1673,7 +1673,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C35" t="s">
         <v>61</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
         <v>62</v>
@@ -1803,19 +1803,19 @@
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>54</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E40" s="17">
         <v>9999</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>11</v>
@@ -1828,13 +1828,13 @@
         <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
         <v>63</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E41" s="3">
         <v>99999</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
         <v>64</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
         <v>65</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
         <v>67</v>
@@ -1902,13 +1902,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
         <v>68</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>91</v>
@@ -1919,13 +1919,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" t="s">
         <v>69</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E46" s="4">
         <v>99999</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C47" t="s">
         <v>70</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
         <v>66</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C50" t="s">
         <v>72</v>
@@ -2020,19 +2020,19 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s">
         <v>73</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E51" s="4">
         <v>99999</v>
       </c>
       <c r="F51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G51" t="s">
         <v>30</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
         <v>75</v>
@@ -2113,7 +2113,7 @@
         <v>77</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E55" s="3">
         <v>999</v>
@@ -2124,13 +2124,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C56" t="s">
         <v>78</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E56" s="3">
         <v>999</v>

</xml_diff>

<commit_message>
Finished operations, added restriction to invAmount
</commit_message>
<xml_diff>
--- a/Autoparts Data Dictionary.xlsx
+++ b/Autoparts Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\GitHub\database-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CC2F0A-A6D0-4267-8668-FFD9CDFAFE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0235538D-EBF7-4AB2-B23D-9A5274BAD61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="142">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -455,6 +455,9 @@
   </si>
   <si>
     <t>&gt;=10000</t>
+  </si>
+  <si>
+    <t>0-9999</t>
   </si>
 </sst>
 </file>
@@ -898,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,6 +1636,9 @@
       <c r="E32" s="3">
         <v>9999</v>
       </c>
+      <c r="F32" t="s">
+        <v>141</v>
+      </c>
       <c r="G32" t="s">
         <v>11</v>
       </c>

</xml_diff>